<commit_message>
- Added Falllback for Database Location - Changed Message for Submitting Form Request
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JC Rosuelo\Desktop\DocumentRequesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JC Rosuelo\source\repos\DocumentRequesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDFCB7B-3541-44BB-85CF-A31DDB581DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECA1149-FFA6-417C-85A6-F477EA062A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="8100" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>ReferenceNumber</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Certificate of Registration</t>
   </si>
   <si>
-    <t>11/30/2024 2:00:00 AM</t>
-  </si>
-  <si>
     <t>Archived</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>69</t>
   </si>
   <si>
-    <t>11/16/2024</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -126,12 +120,6 @@
     <t>Transcript of Record</t>
   </si>
   <si>
-    <t>11/9/2024 7:00:00 PM</t>
-  </si>
-  <si>
-    <t>11/8/2024</t>
-  </si>
-  <si>
     <t>2024-11-30 07:39:35.835107300</t>
   </si>
   <si>
@@ -160,6 +148,63 @@
   </si>
   <si>
     <t>bruhhh</t>
+  </si>
+  <si>
+    <t>Diploma</t>
+  </si>
+  <si>
+    <t>2024-11-30 19:48:48.154722900</t>
+  </si>
+  <si>
+    <t>ewan</t>
+  </si>
+  <si>
+    <t>haha</t>
+  </si>
+  <si>
+    <t>2024-11-23 19:36:29.247893100</t>
+  </si>
+  <si>
+    <t>6942069</t>
+  </si>
+  <si>
+    <t>johnchristian.rosuelo@gmail.com</t>
+  </si>
+  <si>
+    <t>bahay</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>2024-11-30 02:00:00</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>2024-11-23 19:40:22.607090200</t>
+  </si>
+  <si>
+    <t>OnProcess</t>
+  </si>
+  <si>
+    <t>2024-11-23 19:40:50.880861900</t>
+  </si>
+  <si>
+    <t>ewe</t>
+  </si>
+  <si>
+    <t>2024-11-16 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-11-09 19:00:00</t>
+  </si>
+  <si>
+    <t>2024-11-08 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -534,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,163 +653,322 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>31</v>
+      <c r="M7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>